<commit_message>
Adding 2020-04-06 data and editing main R file
</commit_message>
<xml_diff>
--- a/dcCovid-19DataSummaryToday.xlsx
+++ b/dcCovid-19DataSummaryToday.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="165" windowWidth="15375" windowHeight="7875" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="3810" yWindow="165" windowWidth="15375" windowHeight="7875"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overal Stats" sheetId="1" r:id="rId1"/>
     <sheet name="Total Cases by Ward" sheetId="2" r:id="rId2"/>
     <sheet name="Total Cases by Race" sheetId="3" r:id="rId3"/>
-    <sheet name="Deaths by Race" sheetId="4" r:id="rId4"/>
+    <sheet name="Lives Lost by Race" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="57">
   <si>
     <t>Testing</t>
   </si>
@@ -243,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -266,24 +266,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,11 +595,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF62"/>
+  <dimension ref="A1:AG62"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF63" sqref="AF63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +608,7 @@
     <col min="2" max="2" width="62.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C1" s="1">
         <v>43897</v>
       </c>
@@ -702,8 +699,11 @@
       <c r="AF1" s="1">
         <v>43926</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG1" s="1">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -727,7 +727,7 @@
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -803,8 +803,11 @@
       <c r="AF3">
         <v>7453</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG3">
+        <v>7823</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -901,8 +904,11 @@
       <c r="AF4">
         <v>1097</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG4">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -981,8 +987,11 @@
       <c r="AF5">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1031,11 +1040,14 @@
       <c r="AF6">
         <v>287</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG6">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1078,8 +1090,11 @@
       <c r="AF8">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG8">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1122,8 +1137,11 @@
       <c r="AF9">
         <v>432</v>
       </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG9">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1166,8 +1184,11 @@
       <c r="AF10">
         <v>177</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG10">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -1210,13 +1231,16 @@
       <c r="AF11">
         <v>255</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG11">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1224,7 +1248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1273,8 +1297,11 @@
       <c r="AF15">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1314,8 +1341,11 @@
       <c r="AF16">
         <v>196</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG16">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1355,8 +1385,11 @@
       <c r="AF17">
         <v>196</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1396,13 +1429,16 @@
       <c r="AF18">
         <v>179</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG18">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1451,8 +1487,11 @@
       <c r="AF21">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1492,8 +1531,11 @@
       <c r="AF22">
         <v>212</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG22">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1533,8 +1575,11 @@
       <c r="AF23">
         <v>235</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG23">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -1574,13 +1619,16 @@
       <c r="AF24">
         <v>204</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG24">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -1620,8 +1668,11 @@
       <c r="AF27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -1661,8 +1712,11 @@
       <c r="AF28">
         <v>137</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG28">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1702,8 +1756,11 @@
       <c r="AF29">
         <v>141</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG29">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -1743,13 +1800,16 @@
       <c r="AF30">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
@@ -1792,8 +1852,11 @@
       <c r="AF33">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>19</v>
       </c>
@@ -1833,8 +1896,11 @@
       <c r="AF34">
         <v>153</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG34">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
@@ -1874,8 +1940,11 @@
       <c r="AF35">
         <v>171</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
@@ -1915,13 +1984,16 @@
       <c r="AF36">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
@@ -1949,8 +2021,11 @@
       <c r="AF39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>21</v>
       </c>
@@ -1978,8 +2053,11 @@
       <c r="AF40">
         <v>66</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG40">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>21</v>
       </c>
@@ -2007,8 +2085,11 @@
       <c r="AF41">
         <v>69</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG41">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>21</v>
       </c>
@@ -2036,8 +2117,11 @@
       <c r="AF42">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>23</v>
       </c>
@@ -2065,8 +2149,11 @@
       <c r="AF44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>23</v>
       </c>
@@ -2094,8 +2181,11 @@
       <c r="AF45">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
@@ -2123,8 +2213,11 @@
       <c r="AF46">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
@@ -2152,13 +2245,16 @@
       <c r="AF47">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
@@ -2183,8 +2279,11 @@
       <c r="AF50">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG50">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>25</v>
       </c>
@@ -2209,8 +2308,11 @@
       <c r="AF51">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG51">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>25</v>
       </c>
@@ -2235,8 +2337,11 @@
       <c r="AF52">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG52">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>35</v>
       </c>
@@ -2261,8 +2366,11 @@
       <c r="AF54">
         <v>14</v>
       </c>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG54">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>35</v>
       </c>
@@ -2287,8 +2395,11 @@
       <c r="AF55">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG55">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>35</v>
       </c>
@@ -2313,8 +2424,11 @@
       <c r="AF56">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG56">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>35</v>
       </c>
@@ -2339,8 +2453,11 @@
       <c r="AF57" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>36</v>
       </c>
@@ -2365,8 +2482,11 @@
       <c r="AF59">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG59">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>36</v>
       </c>
@@ -2391,8 +2511,11 @@
       <c r="AF60">
         <v>95</v>
       </c>
-    </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG60">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>36</v>
       </c>
@@ -2417,8 +2540,11 @@
       <c r="AF61">
         <v>95</v>
       </c>
-    </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG61">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>36</v>
       </c>
@@ -2441,6 +2567,9 @@
         <v>1</v>
       </c>
       <c r="AF62">
+        <v>1</v>
+      </c>
+      <c r="AG62">
         <v>1</v>
       </c>
     </row>
@@ -2452,10 +2581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G11"/>
+  <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2464,7 +2593,7 @@
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>34</v>
       </c>
@@ -2486,8 +2615,11 @@
       <c r="G2" s="9">
         <v>43926</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="9">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -2509,8 +2641,11 @@
       <c r="G3">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -2532,8 +2667,11 @@
       <c r="G4">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -2555,8 +2693,11 @@
       <c r="G5">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -2578,8 +2719,11 @@
       <c r="G6">
         <v>168</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -2601,8 +2745,11 @@
       <c r="G7">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -2624,8 +2771,11 @@
       <c r="G8">
         <v>187</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -2647,8 +2797,11 @@
       <c r="G9">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -2670,8 +2823,11 @@
       <c r="G10">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>41</v>
       </c>
@@ -2692,6 +2848,9 @@
       </c>
       <c r="G11">
         <v>44</v>
+      </c>
+      <c r="H11">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2702,159 +2861,199 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B18"/>
+  <dimension ref="A2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="16" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="14">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="12">
         <v>43926</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="C2" s="9">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="14">
         <v>1097</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="C3">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="13"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="B4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="14">
         <v>349</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="C5">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="14">
         <v>135</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="C6">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="14">
         <v>303</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="C7">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="14">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="C8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="14">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="C10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="14">
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="14">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="13"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="14">
         <v>341</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="C14">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="14">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="C15">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="14">
         <v>517</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="C16">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="14">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="14">
         <v>2</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2862,56 +3061,73 @@
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="15">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="9">
         <v>43926</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="9">
+        <v>43927</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="C4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>